<commit_message>
Updated to .Net Core 1.1
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27224"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28315"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6120" yWindow="2780" windowWidth="20380" windowHeight="15820" tabRatio="500"/>
+    <workbookView xWindow="1080" yWindow="460" windowWidth="37320" windowHeight="23540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>EF7</t>
   </si>
@@ -37,15 +37,21 @@
   <si>
     <t>Bulk COPY binary</t>
   </si>
+  <si>
+    <t>.NET Core 1.0.1 - EF Core 1.0.1 - PostgreSQL 1.0.2</t>
+  </si>
+  <si>
+    <t>.NET Core 1.1 - EF Core 1.1.2 - PostgreSQL 1.1.1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000\ &quot;s&quot;"/>
+    <numFmt numFmtId="164" formatCode="0.000\ &quot;s&quot;"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -69,13 +75,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -90,16 +109,46 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -372,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="190" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -384,7 +433,7 @@
     <col min="3" max="3" width="10.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="B1" s="2">
         <v>1000</v>
       </c>
@@ -395,49 +444,131 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B3" s="3">
         <v>0.95060699999999998</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C3" s="3">
         <v>3.5997330000000001</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D3" s="3">
         <v>30.982600000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B4" s="3">
         <v>0.55510999999999999</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C4" s="3">
         <v>5.3789090000000002</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D4" s="3">
         <v>54.205333000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B5" s="3">
         <v>4.4776000000000003E-2</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C5" s="3">
         <v>0.27743000000000001</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D5" s="3">
         <v>3.4068480000000001</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1.151491</v>
+      </c>
+      <c r="C7" s="3">
+        <v>3.9001540000000001</v>
+      </c>
+      <c r="D7" s="3">
+        <v>32.759604000000003</v>
+      </c>
+      <c r="E7" s="5">
+        <f>AVERAGE(B7/B3,C7/C3,D7/D3)-1</f>
+        <v>0.11737772949342484</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.56940000000000002</v>
+      </c>
+      <c r="C8" s="3">
+        <v>5.2858080000000003</v>
+      </c>
+      <c r="D8" s="3">
+        <v>52.949038999999999</v>
+      </c>
+      <c r="E8" s="5">
+        <f>AVERAGE(B8/B4,C8/C4,D8/D4)-1</f>
+        <v>-4.9141528608425133E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="3">
+        <v>4.4706000000000003E-2</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.27359</v>
+      </c>
+      <c r="D9" s="3">
+        <v>3.3035169999999998</v>
+      </c>
+      <c r="E9" s="5">
+        <f>AVERAGE(B9/B5,C9/C5,D9/D5)-1</f>
+        <v>-1.524501615930729E-2</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A6:D6"/>
+  </mergeCells>
+  <conditionalFormatting sqref="E7:E9">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>